<commit_message>
Enhance user settings and access control for admin roles; update welcome message and export functionality
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -408,6 +408,7 @@
     <col min="4" max="4" width="20.83203125" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" customWidth="1"/>
     <col min="6" max="6" width="20.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -429,30 +430,36 @@
       <c r="F1" t="str">
         <v>Société</v>
       </c>
+      <c r="G1" t="str">
+        <v>Role</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>zulabejyla@mailinator.com</v>
+        <v>fyzidejiwi@mailinator.com</v>
       </c>
       <c r="B2" t="str">
-        <v>zulabejyla@mailinator.com</v>
+        <v>fyzidejiwi@mailinator.com</v>
       </c>
       <c r="C2" t="str">
-        <v>Eu id similique pla</v>
+        <v>Reiciendis id dolor</v>
       </c>
       <c r="D2" t="str">
-        <v xml:space="preserve">Quia adipisci autem </v>
+        <v>Tenetur blanditiis i</v>
       </c>
       <c r="E2" t="str">
-        <v>+1 (643) 289-7597</v>
+        <v>+1 (411) 862-1585</v>
       </c>
       <c r="F2" t="str">
-        <v xml:space="preserve">Velit veniam magna </v>
+        <v>Fuga Et in distinct</v>
+      </c>
+      <c r="G2" t="str">
+        <v>admin</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enhance index.html: Add ticket data upload functionality and improve user prompts; update toast notifications for better user experience.
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Email</t>
   </si>
@@ -58,7 +58,28 @@
     <t>AniMaro</t>
   </si>
   <si>
-    <t>user</t>
+    <t>User</t>
+  </si>
+  <si>
+    <t>nyzopixu@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minim dolore dolore </t>
+  </si>
+  <si>
+    <t>Adipisicing labore a</t>
+  </si>
+  <si>
+    <t>VOLUPTATES SUSCIPIT</t>
+  </si>
+  <si>
+    <t>+1 (165) 371-6338</t>
+  </si>
+  <si>
+    <t>Excepturi dicta omni</t>
+  </si>
+  <si>
+    <t>dmine</t>
   </si>
 </sst>
 </file>
@@ -405,7 +426,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -473,6 +494,32 @@
         <v>14</v>
       </c>
     </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>